<commit_message>
c lohkon vikat pelit
</commit_message>
<xml_diff>
--- a/Data/11oikearivi.xlsx
+++ b/Data/11oikearivi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedu\Documents\GitHub\euro22\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D432A05-DEAA-4F34-AE3F-932EAD662644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668D2115-DFEF-4DB0-A545-C9716A7D913A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,11 +1860,15 @@
       <c r="E26" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="29"/>
+      <c r="F26" s="29">
+        <v>1</v>
+      </c>
       <c r="G26" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="29"/>
+      <c r="H26" s="29">
+        <v>4</v>
+      </c>
       <c r="J26" s="37" t="s">
         <v>102</v>
       </c>
@@ -1891,11 +1895,15 @@
       <c r="E27" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="29"/>
+      <c r="F27" s="29">
+        <v>5</v>
+      </c>
       <c r="G27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="29">
+        <v>0</v>
+      </c>
       <c r="J27" s="38" t="s">
         <v>69</v>
       </c>
@@ -2143,7 +2151,7 @@
         <v>77</v>
       </c>
       <c r="L41" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
usa-wal ja 2 lappua
</commit_message>
<xml_diff>
--- a/Data/11oikearivi.xlsx
+++ b/Data/11oikearivi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
   <si>
     <t xml:space="preserve">KISAVEIKKAUS</t>
   </si>
@@ -189,10 +189,16 @@
     <t xml:space="preserve">Costa Rica</t>
   </si>
   <si>
+    <t xml:space="preserve">Gareth Bale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belgia</t>
   </si>
   <si>
     <t xml:space="preserve">Kanada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timothy Weah</t>
   </si>
   <si>
     <t xml:space="preserve">G</t>
@@ -503,10 +509,10 @@
   <dimension ref="A1:V127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.67"/>
@@ -728,11 +734,15 @@
       <c r="E9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="G9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="J9" s="20" t="s">
         <v>29</v>
       </c>
@@ -911,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="15" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
         <v>49</v>
       </c>
@@ -932,8 +942,14 @@
         <v>16</v>
       </c>
       <c r="H16" s="18"/>
-    </row>
-    <row r="17" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="15" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
         <v>45</v>
       </c>
@@ -941,35 +957,41 @@
         <v>44888</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="18"/>
+      <c r="J17" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="17" t="s">
@@ -979,19 +1001,19 @@
     </row>
     <row r="19" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B19" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="17" t="s">
@@ -1001,19 +1023,19 @@
     </row>
     <row r="20" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="17" t="s">
@@ -1023,19 +1045,19 @@
     </row>
     <row r="21" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B21" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="17" t="s">
@@ -1249,7 +1271,7 @@
         <v>44892</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>16</v>
@@ -1277,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="17" t="s">
@@ -1309,19 +1331,19 @@
     </row>
     <row r="34" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="17" t="s">
@@ -1331,19 +1353,19 @@
     </row>
     <row r="35" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B35" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="17" t="s">
@@ -1353,19 +1375,19 @@
     </row>
     <row r="36" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B36" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="17" t="s">
@@ -1375,19 +1397,19 @@
     </row>
     <row r="37" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B37" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C37" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>61</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="17" t="s">
@@ -1585,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F46" s="18"/>
       <c r="G46" s="17" t="s">
@@ -1601,7 +1623,7 @@
         <v>44896</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>16</v>
@@ -1661,19 +1683,19 @@
     </row>
     <row r="50" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B50" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="17" t="s">
@@ -1683,19 +1705,19 @@
     </row>
     <row r="51" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B51" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="17" t="s">
@@ -1705,19 +1727,19 @@
     </row>
     <row r="52" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B52" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="17" t="s">
@@ -1727,19 +1749,19 @@
     </row>
     <row r="53" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="17" t="s">
@@ -1826,7 +1848,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1849,7 +1871,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
58 veikkausta ja tan-tun
</commit_message>
<xml_diff>
--- a/Data/11oikearivi.xlsx
+++ b/Data/11oikearivi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="72">
   <si>
     <t xml:space="preserve">KISAVEIKKAUS</t>
   </si>
@@ -210,6 +210,9 @@
     <t xml:space="preserve">Kamerun</t>
   </si>
   <si>
+    <t xml:space="preserve">Lionel Messi</t>
+  </si>
+  <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
@@ -219,10 +222,16 @@
     <t xml:space="preserve">Etelä-Korea</t>
   </si>
   <si>
+    <t xml:space="preserve">Saleh Al-Shehri</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portugali</t>
   </si>
   <si>
     <t xml:space="preserve">Ghana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salem Al Dawsari</t>
   </si>
   <si>
     <t xml:space="preserve">Brasilia</t>
@@ -509,10 +518,10 @@
   <dimension ref="A1:V127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.67"/>
@@ -768,11 +777,15 @@
       <c r="E10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="G10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="18"/>
+      <c r="H10" s="18" t="n">
+        <v>2</v>
+      </c>
       <c r="J10" s="20" t="s">
         <v>34</v>
       </c>
@@ -797,11 +810,15 @@
       <c r="E11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="J11" s="15" t="s">
         <v>38</v>
       </c>
@@ -998,50 +1015,68 @@
         <v>16</v>
       </c>
       <c r="H18" s="18"/>
-    </row>
-    <row r="19" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" s="15" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="18"/>
-    </row>
-    <row r="20" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="15" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="16" t="n">
         <v>44889</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="18"/>
+      <c r="J20" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
@@ -1051,13 +1086,13 @@
         <v>44889</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="17" t="s">
@@ -1343,7 +1378,7 @@
         <v>16</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="17" t="s">
@@ -1353,19 +1388,19 @@
     </row>
     <row r="35" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="17" t="s">
@@ -1381,7 +1416,7 @@
         <v>44893</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>16</v>
@@ -1397,19 +1432,19 @@
     </row>
     <row r="37" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B37" s="16" t="n">
         <v>44893</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="17" t="s">
@@ -1683,19 +1718,19 @@
     </row>
     <row r="50" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B50" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="17" t="s">
@@ -1705,19 +1740,19 @@
     </row>
     <row r="51" s="15" customFormat="true" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B51" s="16" t="n">
         <v>44897</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="17" t="s">
@@ -1733,7 +1768,7 @@
         <v>44897</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>16</v>
@@ -1761,7 +1796,7 @@
         <v>16</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="17" t="s">
@@ -1848,7 +1883,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1871,7 +1906,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>